<commit_message>
PGS update to architecture and spring backlog dogs
</commit_message>
<xml_diff>
--- a/documents/Deliverable_3/FlyingMongeese_Deliverable_3_SprintBacklog.xlsx
+++ b/documents/Deliverable_3/FlyingMongeese_Deliverable_3_SprintBacklog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur Bhakta\Documents\GitHub\Software2project\documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/GitHub/Software2project/documents/Deliverable_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF64DAEB-7925-469D-804D-5C3E408E1286}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="432" windowWidth="22740" windowHeight="15552" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="440" windowWidth="22740" windowHeight="15560" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SprintBacklog1" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="SprintBacklog4" sheetId="5" r:id="rId4"/>
     <sheet name="SprintBacklog5" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="116">
   <si>
     <t>Story Type</t>
   </si>
@@ -531,7 +530,7 @@
     <t>Cade:
 Andre:
 Turner:
-Mayur:X
+Mayur:
 Riggs:
 Carolyn:X</t>
   </si>
@@ -541,17 +540,6 @@
 Turner:
 Mayur:
 Riggs:
-Carolyn:X</t>
-  </si>
-  <si>
-    <t>architecture design and design patterns</t>
-  </si>
-  <si>
-    <t>Cade:
-Andre:
-Turner:
-Mayur:
-Riggs:
 Carolyn: X</t>
   </si>
   <si>
@@ -604,12 +592,42 @@
   </si>
   <si>
     <t>Create retrieval method to get data our of the database</t>
+  </si>
+  <si>
+    <t>Create and update function to return sales for an specific day and show results on the App.</t>
+  </si>
+  <si>
+    <t>Cade:
+Andre:
+Turner:2
+Mayur:2
+Riggs:
+Carolyn:</t>
+  </si>
+  <si>
+    <t>Cade:
+Andre:
+Turner:X
+Mayur:
+Riggs:X
+Carolyn:</t>
+  </si>
+  <si>
+    <t>Architecture Design and Design Patterns</t>
+  </si>
+  <si>
+    <t>Cade:
+Andre:
+Turner:X
+Mayur:
+Riggs:
+Carolyn: X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -674,29 +692,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -704,23 +722,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -827,14 +845,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1200,31 +1218,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1250,7 +1268,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
         <v>10</v>
       </c>
@@ -1273,7 +1291,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A4" s="6">
         <v>11</v>
       </c>
@@ -1296,7 +1314,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A5" s="6">
         <v>12</v>
       </c>
@@ -1319,7 +1337,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A6" s="6">
         <v>13</v>
       </c>
@@ -1342,7 +1360,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A7" s="6">
         <v>14</v>
       </c>
@@ -1365,7 +1383,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A8" s="6">
         <v>15</v>
       </c>
@@ -1390,7 +1408,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A9" s="6">
         <v>16</v>
       </c>
@@ -1415,7 +1433,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A10" s="6">
         <v>17</v>
       </c>
@@ -1440,7 +1458,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A11" s="6">
         <v>18</v>
       </c>
@@ -1463,7 +1481,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A12" s="6">
         <v>19</v>
       </c>
@@ -1486,7 +1504,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A13" s="6">
         <v>20</v>
       </c>
@@ -1511,12 +1529,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="9" t="s">
         <v>31</v>
@@ -1527,7 +1545,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="78" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="9" t="s">
         <v>32</v>
@@ -1544,7 +1562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="9" t="s">
         <v>33</v>
@@ -1561,7 +1579,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="9" t="s">
         <v>34</v>
@@ -1578,7 +1596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="9" t="s">
         <v>38</v>
@@ -1595,7 +1613,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="9" t="s">
         <v>39</v>
@@ -1612,7 +1630,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="9" t="s">
         <v>40</v>
@@ -1629,7 +1647,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1643,10 +1661,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B24" s="3"/>
     </row>
   </sheetData>
@@ -1664,26 +1682,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="7" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="7" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:11" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>12</v>
       </c>
@@ -1709,7 +1727,7 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>10</v>
       </c>
@@ -1734,7 +1752,7 @@
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
     </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>11</v>
       </c>
@@ -1759,7 +1777,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
     </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="12" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A5" s="23">
         <v>12</v>
       </c>
@@ -1782,7 +1800,7 @@
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>13</v>
       </c>
@@ -1805,7 +1823,7 @@
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>14</v>
       </c>
@@ -1828,7 +1846,7 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
     </row>
-    <row r="8" spans="1:11" s="12" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>15</v>
       </c>
@@ -1853,7 +1871,7 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>16</v>
       </c>
@@ -1878,7 +1896,7 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>17</v>
       </c>
@@ -1903,7 +1921,7 @@
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>18</v>
       </c>
@@ -1926,7 +1944,7 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
-    <row r="12" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>20</v>
       </c>
@@ -1951,12 +1969,12 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:11" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:11" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+      <c r="A13" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="38" t="s">
         <v>31</v>
@@ -1971,13 +1989,13 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="23"/>
       <c r="F15" s="26" t="s">
         <v>75</v>
@@ -1986,13 +2004,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="23"/>
       <c r="F16" s="26" t="s">
         <v>4</v>
@@ -2001,13 +2019,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="18" t="s">
         <v>49</v>
       </c>
@@ -2018,13 +2036,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="23"/>
       <c r="F18" s="26" t="s">
         <v>4</v>
@@ -2033,13 +2051,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="27" t="s">
         <v>44</v>
       </c>
@@ -2050,13 +2068,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="23"/>
       <c r="F20" s="26" t="s">
         <v>4</v>
@@ -2065,13 +2083,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="23"/>
       <c r="F21" s="26" t="s">
         <v>4</v>
@@ -2080,13 +2098,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="23"/>
       <c r="F22" s="26" t="s">
         <v>4</v>
@@ -2095,13 +2113,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="23" t="s">
         <v>48</v>
       </c>
@@ -2114,18 +2132,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A13:XFD13"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
     <cfRule type="notContainsBlanks" dxfId="3" priority="1">
@@ -2138,29 +2156,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9D4EE-EF66-4647-A07F-23214E7A01E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -2183,7 +2201,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -2202,7 +2220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>11</v>
       </c>
@@ -2221,7 +2239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>12</v>
       </c>
@@ -2240,7 +2258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>13</v>
       </c>
@@ -2259,7 +2277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>15</v>
       </c>
@@ -2297,7 +2315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -2316,7 +2334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>17</v>
       </c>
@@ -2335,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>18</v>
       </c>
@@ -2354,7 +2372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>19</v>
       </c>
@@ -2373,7 +2391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>20</v>
       </c>
@@ -2392,23 +2410,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:7" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+      <c r="A14" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-    </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="38" t="s">
         <v>32</v>
@@ -2425,7 +2443,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="38" t="s">
         <v>33</v>
@@ -2442,7 +2460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="38" t="s">
         <v>61</v>
@@ -2459,7 +2477,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="38" t="s">
         <v>38</v>
@@ -2476,7 +2494,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="38" t="s">
         <v>39</v>
@@ -2493,7 +2511,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="38" t="s">
         <v>35</v>
@@ -2510,7 +2528,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="38" t="s">
         <v>37</v>
@@ -2527,7 +2545,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="38" t="s">
         <v>36</v>
@@ -2544,7 +2562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="38" t="s">
         <v>40</v>
@@ -2561,16 +2579,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A14:XFD14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B24:D24"/>
@@ -2578,11 +2601,6 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="A1:XFD1"/>
-    <mergeCell ref="A14:XFD14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2">
     <cfRule type="notContainsBlanks" dxfId="2" priority="1">
@@ -2595,29 +2613,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD0DEDB-7184-4D60-B99A-9BCC4CFD825C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" style="3" customWidth="1"/>
     <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -2640,7 +2658,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -2661,7 +2679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>11</v>
       </c>
@@ -2676,13 +2694,13 @@
         <v>98</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>12</v>
       </c>
@@ -2703,7 +2721,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>13</v>
       </c>
@@ -2722,7 +2740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -2741,7 +2759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>15</v>
       </c>
@@ -2762,7 +2780,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -2783,7 +2801,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>17</v>
       </c>
@@ -2804,7 +2822,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>18</v>
       </c>
@@ -2816,7 +2834,7 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>52</v>
@@ -2825,7 +2843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>19</v>
       </c>
@@ -2844,7 +2862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>20</v>
       </c>
@@ -2863,7 +2881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>21</v>
       </c>
@@ -2882,26 +2900,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:7" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+    <row r="16" spans="1:7" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+      <c r="A16" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-    </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+    </row>
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="38" t="s">
         <v>32</v>
@@ -2918,7 +2936,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="38" t="s">
         <v>33</v>
@@ -2935,7 +2953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="38" t="s">
         <v>61</v>
@@ -2952,7 +2970,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="38" t="s">
         <v>38</v>
@@ -2969,7 +2987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="38" t="s">
         <v>39</v>
@@ -2986,7 +3004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="38" t="s">
         <v>35</v>
@@ -2997,13 +3015,13 @@
         <v>49</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="38" t="s">
         <v>37</v>
@@ -3020,7 +3038,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="38" t="s">
         <v>36</v>
@@ -3037,7 +3055,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="38" t="s">
         <v>40</v>
@@ -3048,15 +3066,15 @@
         <v>48</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="96" x14ac:dyDescent="0.15">
       <c r="B27" s="38" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="40"/>
@@ -3064,13 +3082,13 @@
         <v>49</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E28"/>
     </row>
   </sheetData>
@@ -3100,29 +3118,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB03CE47-C0CE-41ED-B770-BE9613398E6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" customWidth="1"/>
     <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="36" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -3145,7 +3163,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -3166,7 +3184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>11</v>
       </c>
@@ -3181,13 +3199,13 @@
         <v>98</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>12</v>
       </c>
@@ -3202,13 +3220,13 @@
         <v>94</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>13</v>
       </c>
@@ -3227,7 +3245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>14</v>
       </c>
@@ -3246,7 +3264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>15</v>
       </c>
@@ -3258,16 +3276,16 @@
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -3282,13 +3300,13 @@
         <v>99</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>17</v>
       </c>
@@ -3303,13 +3321,13 @@
         <v>101</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>18</v>
       </c>
@@ -3321,7 +3339,7 @@
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>74</v>
@@ -3330,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>19</v>
       </c>
@@ -3349,7 +3367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>20</v>
       </c>
@@ -3368,7 +3386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
         <v>84</v>
@@ -3383,23 +3401,23 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+    <row r="15" spans="1:7" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.15">
+      <c r="A15" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-    </row>
-    <row r="17" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="38" t="s">
         <v>32</v>
@@ -3416,7 +3434,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="38" t="s">
         <v>33</v>
@@ -3433,7 +3451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="38" t="s">
         <v>61</v>
@@ -3450,7 +3468,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="38" t="s">
         <v>38</v>
@@ -3467,7 +3485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="38" t="s">
         <v>39</v>
@@ -3484,7 +3502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="38" t="s">
         <v>35</v>
@@ -3495,16 +3513,16 @@
         <v>49</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="38" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="40"/>
@@ -3512,13 +3530,13 @@
         <v>49</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="38" t="s">
         <v>36</v>
@@ -3529,13 +3547,13 @@
         <v>49</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="G24" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="38" t="s">
         <v>40</v>
@@ -3546,13 +3564,13 @@
         <v>48</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="96" x14ac:dyDescent="0.15">
       <c r="A26" s="20"/>
       <c r="B26" s="38" t="s">
         <v>87</v>
@@ -3569,9 +3587,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="93.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="96" x14ac:dyDescent="0.15">
       <c r="B27" s="38" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="40"/>
@@ -3579,10 +3597,10 @@
         <v>49</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>